<commit_message>
Commit 30.1: SAving Local Changes for Robot
</commit_message>
<xml_diff>
--- a/References/Selenium Cheatsheets/XPath-CSSSelector Mind Map.xlsx
+++ b/References/Selenium Cheatsheets/XPath-CSSSelector Mind Map.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/939c1bf4b082bbe3/Desktop/Projects/Testing Projects/Python-Pytest-Robot/Automation-Testing-with-Python/References/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/939c1bf4b082bbe3/Desktop/Projects/Testing Projects/Python-Pytest-Robot/Automation-Testing-with-Python/References/Selenium Cheatsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_21C89FCDF21DFB95F0994269EDE04F4AB30EF49B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7A2BE2C-851C-4BBF-A18A-05B904E5E669}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_21C89FCDF21DFB95F0994269EDE04F4AB30EF49B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{115C1F32-A29A-44E3-90D8-7D48FD0DC5E5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="234">
   <si>
     <t>Selector Type</t>
   </si>
@@ -1716,16 +1716,13 @@
   </si>
   <si>
     <t>XPath Selector Cheat Sheet: Practical Examples Included</t>
-  </si>
-  <si>
-    <t>--</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1780,6 +1777,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1809,7 +1811,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1826,24 +1828,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1860,6 +1863,2524 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>485775</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1027" name="Check Box 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1027"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1028" name="Check Box 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33BDE6D0-3E27-471B-AE0D-0672DE2DAFF3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="Check Box 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E590278C-81F6-48FE-8378-CE7847F92D25}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1030" name="Check Box 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1030"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F63BA49-4D17-461A-AC39-D0A3DBE4315B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1031" name="Check Box 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1031"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7BD22D7-C22A-479F-96F4-7800870BE248}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1032" name="Check Box 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1032"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8208967-4308-47A1-8A4F-F33767D78B35}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1033" name="Check Box 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1033"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{160FFE23-5579-4098-9490-B8FE8B45C1AE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1034" name="Check Box 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1034"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3136BD4-F838-447D-AF68-9D37C37FDAF1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1035" name="Check Box 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1035"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F20BAC7-DE22-4FD5-8D30-B804D1199EE0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1036" name="Check Box 12" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1036"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB2F15F3-5E28-497F-AB7B-EA9EDDD1F06B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1037" name="Check Box 13" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1037"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8C4EE33-BE68-464D-B04B-CC9200E7BE59}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1038" name="Check Box 14" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1038"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBDF4628-E298-4561-8981-38AE9091DA15}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1039" name="Check Box 15" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1039"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0F71163-DF1B-489F-9526-ED56064AB402}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1040" name="Check Box 16" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1040"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F48712FD-1CC1-4825-87A6-806D02D07E74}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1041" name="Check Box 17" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1041"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EFAC012-FBED-40E6-A221-B912C1029C6F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1042" name="Check Box 18" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1042"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D7E16F8-D60D-49AC-95CE-41B3EF83B8F2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1043" name="Check Box 19" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1043"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58BCB8AD-8088-4F6B-A996-BD5B61D11702}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1044" name="Check Box 20" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1044"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AC7DD56-E398-4321-9C94-415D347F8043}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1045" name="Check Box 21" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1045"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4816BB4-A07D-46FF-9F4D-DE7887899A39}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1046" name="Check Box 22" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1046"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF220628-0DEE-49B9-85D0-7FFF268B850D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1047" name="Check Box 23" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1047"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{281533E3-8310-4FD4-B0F6-3E6D3DD38885}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1048" name="Check Box 24" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1048"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC2F3E81-13EF-4632-BB27-981BB701E5BA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1049" name="Check Box 25" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1049"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CE2021A-E360-47E2-B4B8-95DB210BC5C1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1050" name="Check Box 26" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1050"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74AA5BC1-8D41-43CA-A735-925DE26929D3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>25</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1051" name="Check Box 27" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1051"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58A84960-0220-4E89-BC7A-D55C20ED9B57}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1052" name="Check Box 28" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1052"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7ECB1F74-E9D2-4A96-811E-CD22E1067C6B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1053" name="Check Box 29" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1053"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B3C3969-2370-4605-8513-6DD00BD86EF5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1054" name="Check Box 30" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1054"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6BCF256-E367-478E-B9BD-2715C971CA21}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1055" name="Check Box 31" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1055"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEB8AE64-E007-4FBA-BD57-D068180AA613}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>30</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1056" name="Check Box 32" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1056"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BFE27B1-1617-498D-89E5-2F1ABB67BE80}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>31</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1057" name="Check Box 33" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1057"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ACE40A6-6A90-4BBD-BE4A-092A741D5DCF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1058" name="Check Box 34" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1058"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C60987B-E874-428F-9731-F0551A807B2D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>33</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1059" name="Check Box 35" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1059"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31DB35B4-A57F-451F-92FE-67887CE3DFE9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>34</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1060" name="Check Box 36" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1060"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CAE5429-3512-4E5B-8F35-0FCE2D35D857}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>35</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1061" name="Check Box 37" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1061"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74E2645B-D6E6-4FA2-B933-B25CDF4D7AA8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>36</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1062" name="Check Box 38" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1062"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6507D9A4-68C7-4F03-9E6C-4D74ED958D1F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>37</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1063" name="Check Box 39" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1063"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B83B906-2F75-496A-9110-AACE42167DE4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>38</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="266700" cy="142875"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1064" name="Check Box 40" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1064"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76282D20-483A-4E1E-9408-D9843CF9F7EE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2592,25 +5113,25 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="8" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="9" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="9" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="9" t="s">
         <v>233</v>
       </c>
     </row>
@@ -2626,21 +5147,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26442553-F444-4F23-A1B8-3E7BEDE365E5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26442553-F444-4F23-A1B8-3E7BEDE365E5}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2661,485 +5182,1364 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>234</v>
-      </c>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="9"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>120</v>
       </c>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="9"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>123</v>
       </c>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="9"/>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>126</v>
       </c>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="9"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>129</v>
       </c>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="9"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>132</v>
       </c>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>136</v>
       </c>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="9"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>139</v>
       </c>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="9"/>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>142</v>
       </c>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="9"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>145</v>
       </c>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="9"/>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="10"/>
+      <c r="B12" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>148</v>
       </c>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="9"/>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>151</v>
       </c>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="9"/>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="10"/>
+      <c r="B14" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>154</v>
       </c>
+      <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>158</v>
       </c>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="9"/>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>161</v>
       </c>
+      <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="9"/>
-      <c r="B17" s="7" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" s="10"/>
+      <c r="B17" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="E17" s="11"/>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="9"/>
-      <c r="B18" s="7" t="s">
+    <row r="18" spans="1:5">
+      <c r="A18" s="10"/>
+      <c r="B18" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>167</v>
       </c>
+      <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="9"/>
-      <c r="B19" s="7" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" s="10"/>
+      <c r="B19" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>170</v>
       </c>
+      <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="9"/>
-      <c r="B20" s="7" t="s">
+    <row r="20" spans="1:5">
+      <c r="A20" s="10"/>
+      <c r="B20" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>173</v>
       </c>
+      <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="9"/>
-      <c r="B21" s="7" t="s">
+    <row r="21" spans="1:5">
+      <c r="A21" s="10"/>
+      <c r="B21" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>176</v>
       </c>
+      <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="9"/>
-      <c r="B22" s="7" t="s">
+    <row r="22" spans="1:5">
+      <c r="A22" s="10"/>
+      <c r="B22" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>178</v>
       </c>
+      <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="9" t="s">
+    <row r="23" spans="1:5">
+      <c r="A23" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>181</v>
       </c>
+      <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="9"/>
-      <c r="B24" s="7" t="s">
+    <row r="24" spans="1:5">
+      <c r="A24" s="10"/>
+      <c r="B24" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>184</v>
       </c>
+      <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="9"/>
-      <c r="B25" s="7" t="s">
+    <row r="25" spans="1:5">
+      <c r="A25" s="10"/>
+      <c r="B25" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>187</v>
       </c>
+      <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="9" t="s">
+    <row r="26" spans="1:5">
+      <c r="A26" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="6" t="s">
         <v>191</v>
       </c>
+      <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="9"/>
-      <c r="B27" s="7" t="s">
+    <row r="27" spans="1:5">
+      <c r="A27" s="10"/>
+      <c r="B27" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>194</v>
       </c>
+      <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="9"/>
-      <c r="B28" s="7" t="s">
+    <row r="28" spans="1:5">
+      <c r="A28" s="10"/>
+      <c r="B28" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>197</v>
       </c>
+      <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="9"/>
-      <c r="B29" s="7" t="s">
+    <row r="29" spans="1:5">
+      <c r="A29" s="10"/>
+      <c r="B29" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>151</v>
       </c>
+      <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="9"/>
-      <c r="B30" s="7" t="s">
+    <row r="30" spans="1:5">
+      <c r="A30" s="10"/>
+      <c r="B30" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>201</v>
       </c>
+      <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="9"/>
-      <c r="B31" s="7" t="s">
+    <row r="31" spans="1:5">
+      <c r="A31" s="10"/>
+      <c r="B31" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>204</v>
       </c>
+      <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="9"/>
-      <c r="B32" s="7" t="s">
+    <row r="32" spans="1:5">
+      <c r="A32" s="10"/>
+      <c r="B32" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="6" t="s">
         <v>207</v>
       </c>
+      <c r="E32" s="11"/>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="9"/>
-      <c r="B33" s="7" t="s">
+    <row r="33" spans="1:5">
+      <c r="A33" s="10"/>
+      <c r="B33" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="6" t="s">
         <v>210</v>
       </c>
+      <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="9"/>
-      <c r="B34" s="7" t="s">
+    <row r="34" spans="1:5">
+      <c r="A34" s="10"/>
+      <c r="B34" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="6" t="s">
         <v>213</v>
       </c>
+      <c r="E34" s="11"/>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="9"/>
-      <c r="B35" s="7" t="s">
+    <row r="35" spans="1:5">
+      <c r="A35" s="10"/>
+      <c r="B35" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="6" t="s">
         <v>216</v>
       </c>
+      <c r="E35" s="11"/>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="9"/>
-      <c r="B36" s="7" t="s">
+    <row r="36" spans="1:5">
+      <c r="A36" s="10"/>
+      <c r="B36" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="6" t="s">
         <v>219</v>
       </c>
+      <c r="E36" s="11"/>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="9" t="s">
+    <row r="37" spans="1:5">
+      <c r="A37" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="7" t="s">
         <v>223</v>
       </c>
+      <c r="E37" s="11"/>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="9"/>
-      <c r="B38" s="8" t="s">
+    <row r="38" spans="1:5">
+      <c r="A38" s="10"/>
+      <c r="B38" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="7" t="s">
         <v>225</v>
       </c>
+      <c r="E38" s="11"/>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="9"/>
-      <c r="B39" s="8" t="s">
+    <row r="39" spans="1:5">
+      <c r="A39" s="10"/>
+      <c r="B39" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="7" t="s">
         <v>228</v>
       </c>
+      <c r="E39" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A37:A39"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A14"/>
     <mergeCell ref="A15:A22"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A26:A36"/>
-    <mergeCell ref="A37:A39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1027" r:id="rId3" name="Check Box 3">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1028" r:id="rId4" name="Check Box 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1029" r:id="rId5" name="Check Box 5">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1030" r:id="rId6" name="Check Box 6">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1031" r:id="rId7" name="Check Box 7">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1032" r:id="rId8" name="Check Box 8">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1033" r:id="rId9" name="Check Box 9">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1034" r:id="rId10" name="Check Box 10">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1035" r:id="rId11" name="Check Box 11">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1036" r:id="rId12" name="Check Box 12">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1037" r:id="rId13" name="Check Box 13">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1038" r:id="rId14" name="Check Box 14">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1039" r:id="rId15" name="Check Box 15">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1040" r:id="rId16" name="Check Box 16">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1041" r:id="rId17" name="Check Box 17">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1042" r:id="rId18" name="Check Box 18">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1043" r:id="rId19" name="Check Box 19">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1044" r:id="rId20" name="Check Box 20">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1045" r:id="rId21" name="Check Box 21">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1046" r:id="rId22" name="Check Box 22">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1047" r:id="rId23" name="Check Box 23">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>21</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>21</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1048" r:id="rId24" name="Check Box 24">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>22</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>22</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1049" r:id="rId25" name="Check Box 25">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>23</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>23</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1050" r:id="rId26" name="Check Box 26">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>24</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>24</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1051" r:id="rId27" name="Check Box 27">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>25</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>25</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1052" r:id="rId28" name="Check Box 28">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>26</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>26</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1053" r:id="rId29" name="Check Box 29">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>27</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>27</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1054" r:id="rId30" name="Check Box 30">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>28</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>28</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1055" r:id="rId31" name="Check Box 31">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>29</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>29</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1056" r:id="rId32" name="Check Box 32">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>30</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>30</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1057" r:id="rId33" name="Check Box 33">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>31</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>31</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1058" r:id="rId34" name="Check Box 34">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>32</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>32</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1059" r:id="rId35" name="Check Box 35">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>33</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>33</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1060" r:id="rId36" name="Check Box 36">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>34</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>34</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1061" r:id="rId37" name="Check Box 37">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>35</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>35</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1062" r:id="rId38" name="Check Box 38">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>36</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>36</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1063" r:id="rId39" name="Check Box 39">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>37</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>37</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1064" r:id="rId40" name="Check Box 40">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>38</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>485775</xdr:colOff>
+                    <xdr:row>38</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>